<commit_message>
The Last Update 2024-02-21
</commit_message>
<xml_diff>
--- a/enviar_whatsapp/Enviar.xlsx
+++ b/enviar_whatsapp/Enviar.xlsx
@@ -160,7 +160,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.45"/>
   </cols>
@@ -184,7 +184,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45354</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -195,7 +195,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45354</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>